<commit_message>
[#9] update ddl for auto increment in primary key
</commit_message>
<xml_diff>
--- a/Docs/DB/ERD.xlsx
+++ b/Docs/DB/ERD.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ERD 1.0.0" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DDL 1.0.0" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DDL 1.0.1" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DDL 1.0.0" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,44 +13,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>CREATE TABLE `tb_comment` (
+  `C_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '댓글 SEQ',
+  `COMMENT` varchar(1000) DEFAULT NULL COMMENT '댓글 내용',
+  `P_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '대댓글 용 부모 ID,\r\nNULL : 원글\r\nNOT NULL : 부모 댓글 SEQ',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  `VIEW` tinyint(1) NOT NULL DEFAULT '0' COMMENT '노출, 미사용 FLAG\r\n0 : 비노출, 미사용, False\r\n1 : 노출, 사용, True',
+  `U_SEQ` mediumint(9) unsigned NOT NULL COMMENT '사용자 시퀀스 ID',
+  `O_SEQ` mediumint(9) unsigned NOT NULL COMMENT '주문 시퀀스',
+  PRIMARY KEY (`C_SEQ`),
+  KEY `FK_TB_ORDER_TO_TB_COMMENT_1` (`O_SEQ`),
+  KEY `FK_TB_USER_TO_TB_COMMENT_1` (`U_SEQ`),
+  CONSTRAINT `FK_TB_ORDER_TO_TB_COMMENT_1` FOREIGN KEY (`O_SEQ`) REFERENCES `tb_order` (`O_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_USER_TO_TB_COMMENT_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_menu definition
+CREATE TABLE `tb_menu` (
+  `M_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '메뉴 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '메뉴 이름',
+  `PRICE` mediumint(8) unsigned NOT NULL DEFAULT '0' COMMENT '메뉴 가격',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `R_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '식당 SEQ',
+  PRIMARY KEY (`M_SEQ`),
+  KEY `FK_TB_RESTAURANT_TO_TB_MENU_1` (`R_SEQ`),
+  CONSTRAINT `FK_TB_RESTAURANT_TO_TB_MENU_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_order definition
+CREATE TABLE `tb_order` (
+  `O_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '주문 시퀀스',
+  `STATUS` enum('ONLINE','OFFLINE','ORDER','ARRIVAL') NOT NULL DEFAULT 'ONLINE' COMMENT '주문 상태, ONLINE : 참여 가능, OFFLINE : 참여 마감, ORDER : 주문 진행, ARRIVAL : 도착 완료',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '주문 생성 일자',
+  `OFFLINE_TIME` timestamp NULL DEFAULT NULL COMMENT '마감 상태(OFFLINE ) 일자',
+  `ORDER_TIME` timestamp NULL DEFAULT NULL COMMENT '주문 상태(ORDER) 일자',
+  `ARRIVAL_TIME` timestamp NULL DEFAULT NULL COMMENT '도착 상태(ARRIVAL) 일자',
+  `R_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '식당 SEQ',
+  PRIMARY KEY (`O_SEQ`),
+  KEY `FK_TB_RESTAURANT_TO_TB_ORDER_1` (`R_SEQ`),
+  CONSTRAINT `FK_TB_RESTAURANT_TO_TB_ORDER_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_restaurant definition
+CREATE TABLE `tb_restaurant` (
+  `R_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '식당 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '식당 이름',
+  `API_ID` varchar(100) DEFAULT NULL COMMENT '요기요 API 식당 식별 ID',
+  `TEL` varchar(100) DEFAULT NULL COMMENT '식당 전화번호',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\nETC : 기타, 없음',
+  PRIMARY KEY (`R_SEQ`)
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_review definition
+CREATE TABLE `tb_review` (
+  `RV_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '후기 SEQ',
+  `LIKE` tinyint(1) NOT NULL DEFAULT '0' COMMENT '좋아요 FLAG\r\n0 : 싫어요, False\r\n1 : 좋아요, True',
+  `COMMENT` varchar(1000) DEFAULT NULL COMMENT '후기 내용',
+  `VIEW` tinyint(1) NOT NULL DEFAULT '0' COMMENT '노출, 미사용 FLAG\r\n0 : 비노출, 미사용, False\r\n1 : 노출, 사용, True',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성일자',
+  `M_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '메뉴 SEQ',
+  PRIMARY KEY (`RV_SEQ`),
+  KEY `FK_TB_MENU_TO_TB_REVIEW_1` (`M_SEQ`),
+  CONSTRAINT `FK_TB_MENU_TO_TB_REVIEW_1` FOREIGN KEY (`M_SEQ`) REFERENCES `tb_menu` (`M_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_user definition
+CREATE TABLE `tb_user` (
+  `U_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 시퀀스 ID',
+  `NICKNAME` varchar(100) DEFAULT NULL COMMENT '사용자 닉네임',
+  `IP` varchar(100) DEFAULT NULL COMMENT 'IP 주소',
+  PRIMARY KEY (`U_SEQ`)
+) ENGINE=InnoDB AUTO_INCREMENT=2 DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_user_order definition
+CREATE TABLE `tb_user_order` (
+  `UO_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 주문 SEQ',
+  `U_SEQ` mediumint(9) unsigned NOT NULL COMMENT '사용자 시퀀스 ID',
+  `O_SEQ` mediumint(9) unsigned NOT NULL COMMENT '주문 시퀀스',
+  `HOST` tinyint(1) NOT NULL DEFAULT '0' COMMENT '원글 작성자 여부 FLAG\r\n0 : 참여자, False\r\n1 : 작성자, True',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  `M_SEQ` mediumint(9) unsigned NOT NULL COMMENT '메뉴 SEQ',
+  `RV_SEQ` mediumint(9) unsigned NOT NULL COMMENT '후기 SEQ',
+  PRIMARY KEY (`UO_SEQ`),
+  KEY `FK_TB_REVIEW_TO_TB_USER_ORDER_1` (`RV_SEQ`),
+  KEY `FK_TB_MENU_TO_TB_USER_ORDER_1` (`M_SEQ`),
+  KEY `FK_TB_ORDER_TO_TB_USER_ORDER_1` (`O_SEQ`),
+  KEY `FK_TB_USER_TO_TB_USER_ORDER_1` (`U_SEQ`),
+  CONSTRAINT `FK_TB_MENU_TO_TB_USER_ORDER_1` FOREIGN KEY (`M_SEQ`) REFERENCES `tb_menu` (`M_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_ORDER_TO_TB_USER_ORDER_1` FOREIGN KEY (`O_SEQ`) REFERENCES `tb_order` (`O_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_REVIEW_TO_TB_USER_ORDER_1` FOREIGN KEY (`RV_SEQ`) REFERENCES `tb_review` (`RV_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_USER_TO_TB_USER_ORDER_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
   <si>
     <t xml:space="preserve">DROP TABLE IF EXISTS `TB_USER`;
 CREATE TABLE `TB_USER` (
-	`U_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '사용자 시퀀스 ID',
-	`NICKNAME`	VARCHAR(100)	NULL	COMMENT '사용자 닉네임',
-	`IP`	VARCHAR(100)	NULL	COMMENT 'IP 주소'
+        `U_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '사용자 시퀀스 ID',
+        `NICKNAME`        VARCHAR(100)        NULL        COMMENT '사용자 닉네임',
+        `IP`        VARCHAR(100)        NULL        COMMENT 'IP 주소'
 );
 DROP TABLE IF EXISTS `TB_ORDER`;
 CREATE TABLE `TB_ORDER` (
-	`O_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '주문 시퀀스',
-	`STATUS`	ENUM('ONLINE', 'OFFLINE', 'ORDER', 'ARRIVAL')	NOT NULL	DEFAULT 'ONLINE'	COMMENT '주문 상태, ONLINE : 참여 가능, OFFLINE : 참여 마감, ORDER : 주문 진행, ARRIVAL : 도착 완료',
-	`CREATED_TIME`	TIMESTAMP	NOT NULL	DEFAULT CURRENT_TIMESTAMP	COMMENT '주문 생성 일자',
-	`OFFLINE_TIME`	TIMESTAMP	NULL	COMMENT '마감 상태(OFFLINE ) 일자',
-	`ORDER_TIME`	TIMESTAMP	NULL	COMMENT '주문 상태(ORDER) 일자',
-	`ARRIVAL_TIME`	TIMESTAMP	NULL	COMMENT '도착 상태(ARRIVAL) 일자',
-	`R_SEQ`	MEDIUMINT(9) UNSIGNED	NULL	COMMENT '식당 SEQ'
+        `O_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '주문 시퀀스',
+        `STATUS`        ENUM('ONLINE', 'OFFLINE', 'ORDER', 'ARRIVAL')        NOT NULL        DEFAULT 'ONLINE'        COMMENT '주문 상태, ONLINE : 참여 가능, OFFLINE : 참여 마감, ORDER : 주문 진행, ARRIVAL : 도착 완료',
+        `CREATED_TIME`        TIMESTAMP        NOT NULL        DEFAULT CURRENT_TIMESTAMP        COMMENT '주문 생성 일자',
+        `OFFLINE_TIME`        TIMESTAMP        NULL        COMMENT '마감 상태(OFFLINE ) 일자',
+        `ORDER_TIME`        TIMESTAMP        NULL        COMMENT '주문 상태(ORDER) 일자',
+        `ARRIVAL_TIME`        TIMESTAMP        NULL        COMMENT '도착 상태(ARRIVAL) 일자',
+        `R_SEQ`        MEDIUMINT(9) UNSIGNED        NULL        COMMENT '식당 SEQ'
 );
 DROP TABLE IF EXISTS `TB_USER_ORDER`;
 CREATE TABLE `TB_USER_ORDER` (
-	`UO_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '사용자 주문 SEQ',
-	`U_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '사용자 시퀀스 ID',
-	`O_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '주문 시퀀스',
-	`HOST`	TINYINT(1)	NOT NULL	DEFAULT 0	COMMENT '원글 작성자 여부 FLAG
+        `UO_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '사용자 주문 SEQ',
+        `U_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '사용자 시퀀스 ID',
+        `O_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '주문 시퀀스',
+        `HOST`        TINYINT(1)        NOT NULL        DEFAULT 0        COMMENT '원글 작성자 여부 FLAG
 0 : 참여자, False
 1 : 작성자, True',
-	`CREATED_TIME`	TIMESTAMP	NULL	DEFAULT CURRENT_TIMESTAMP	COMMENT '생성 일자',
-	`M_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '메뉴 SEQ',
-	`RV_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '후기 SEQ'
+        `CREATED_TIME`        TIMESTAMP        NULL        DEFAULT CURRENT_TIMESTAMP        COMMENT '생성 일자',
+        `M_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '메뉴 SEQ',
+        `RV_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '후기 SEQ'
 );
 DROP TABLE IF EXISTS `TB_RESTAURANT`;
 CREATE TABLE `TB_RESTAURANT` (
-	`R_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '식당 SEQ',
-	`NAME`	VARCHAR(100)	NULL	COMMENT '식당 이름',
-	`API_ID`	VARCHAR(100)	NULL	COMMENT '요기요 API 식당 식별 ID',
-	`TEL`	VARCHAR(100)	NULL	COMMENT '식당 전화번호',
-	`IMG_LINK`	VARCHAR(512)	NULL	COMMENT '요기요 이미지 Link 주소',
-	`CATEGORY`	ENUM('CHINA', 'KOREA', 'JAPAN', 'ALONE', 'FRANCHISE', 'WESTERN', 'PIG', 'NIGHT', 'SCHOOL', 'CAFE', 'MART', 'ETC')	NULL	DEFAULT 'ETC'	COMMENT '식당 카테고리
+        `R_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '식당 SEQ',
+        `NAME`        VARCHAR(100)        NULL        COMMENT '식당 이름',
+        `API_ID`        VARCHAR(100)        NULL        COMMENT '요기요 API 식당 식별 ID',
+        `TEL`        VARCHAR(100)        NULL        COMMENT '식당 전화번호',
+        `IMG_LINK`        VARCHAR(512)        NULL        COMMENT '요기요 이미지 Link 주소',
+        `CATEGORY`        ENUM('CHINA', 'KOREA', 'JAPAN', 'ALONE', 'FRANCHISE', 'WESTERN', 'PIG', 'NIGHT', 'SCHOOL', 'CAFE', 'MART', 'ETC')        NULL        DEFAULT 'ETC'        COMMENT '식당 카테고리
 CHINA : 중식
 KOREA : 한식
 JAPAN : 일식/돈까스
@@ -65,113 +166,113 @@
 );
 DROP TABLE IF EXISTS `TB_MENU`;
 CREATE TABLE `TB_MENU` (
-	`M_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '메뉴 SEQ',
-	`NAME`	VARCHAR(100)	NULL	COMMENT '메뉴 이름',
-	`PRICE`	MEDIUMINT(8) UNSIGNED	NOT NULL	DEFAULT 0	COMMENT '메뉴 가격',
-	`IMG_LINK`	VARCHAR(512)	NULL	COMMENT '요기요 이미지 Link 주소',
-	`R_SEQ`	MEDIUMINT(9) UNSIGNED	NULL	COMMENT '식당 SEQ'
+        `M_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '메뉴 SEQ',
+        `NAME`        VARCHAR(100)        NULL        COMMENT '메뉴 이름',
+        `PRICE`        MEDIUMINT(8) UNSIGNED        NOT NULL        DEFAULT 0        COMMENT '메뉴 가격',
+        `IMG_LINK`        VARCHAR(512)        NULL        COMMENT '요기요 이미지 Link 주소',
+        `R_SEQ`        MEDIUMINT(9) UNSIGNED        NULL        COMMENT '식당 SEQ'
 );
 DROP TABLE IF EXISTS `TB_REVIEW`;
 CREATE TABLE `TB_REVIEW` (
-	`RV_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '후기 SEQ',
-	`LIKE`	TINYINT(1)	NOT NULL	DEFAULT 0	COMMENT '좋아요 FLAG
+        `RV_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '후기 SEQ',
+        `LIKE`        TINYINT(1)        NOT NULL        DEFAULT 0        COMMENT '좋아요 FLAG
 0 : 싫어요, False
 1 : 좋아요, True',
-	`COMMENT`	VARCHAR(1000)	NULL	COMMENT '후기 내용',
-	`VIEW`	TINYINT(1)	NOT NULL	DEFAULT 0	COMMENT '노출, 미사용 FLAG
+        `COMMENT`        VARCHAR(1000)        NULL        COMMENT '후기 내용',
+        `VIEW`        TINYINT(1)        NOT NULL        DEFAULT 0        COMMENT '노출, 미사용 FLAG
 0 : 비노출, 미사용, False
 1 : 노출, 사용, True',
-	`CREATED_TIME`	TIMESTAMP	NULL	DEFAULT CURRENT_TIMESTAMP	COMMENT '생성일자',
-	`M_SEQ`	MEDIUMINT(9) UNSIGNED	NULL	COMMENT '메뉴 SEQ'
+        `CREATED_TIME`        TIMESTAMP        NULL        DEFAULT CURRENT_TIMESTAMP        COMMENT '생성일자',
+        `M_SEQ`        MEDIUMINT(9) UNSIGNED        NULL        COMMENT '메뉴 SEQ'
 );
 DROP TABLE IF EXISTS `TB_COMMENT`;
 CREATE TABLE `TB_COMMENT` (
-	`C_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '댓글 SEQ',
-	`COMMENT`	VARCHAR(1000)	NULL	COMMENT '댓글 내용',
-	`P_SEQ`	MEDIUMINT(9) UNSIGNED	NULL	COMMENT '대댓글 용 부모 ID,
+        `C_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '댓글 SEQ',
+        `COMMENT`        VARCHAR(1000)        NULL        COMMENT '댓글 내용',
+        `P_SEQ`        MEDIUMINT(9) UNSIGNED        NULL        COMMENT '대댓글 용 부모 ID,
 NULL : 원글
 NOT NULL : 부모 댓글 SEQ',
-	`CREATED_TIME`	TIMESTAMP	NULL	DEFAULT CURRENT_TIMESTAMP	COMMENT '생성 일자',
-	`VIEW`	TINYINT(1)	NOT NULL	DEFAULT 0	COMMENT '노출, 미사용 FLAG
+        `CREATED_TIME`        TIMESTAMP        NULL        DEFAULT CURRENT_TIMESTAMP        COMMENT '생성 일자',
+        `VIEW`        TINYINT(1)        NOT NULL        DEFAULT 0        COMMENT '노출, 미사용 FLAG
 0 : 비노출, 미사용, False
 1 : 노출, 사용, True',
-	`U_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '사용자 시퀀스 ID',
-	`O_SEQ`	MEDIUMINT(9) UNSIGNED	NOT NULL	COMMENT '주문 시퀀스'
+        `U_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '사용자 시퀀스 ID',
+        `O_SEQ`        MEDIUMINT(9) UNSIGNED        NOT NULL        COMMENT '주문 시퀀스'
 );
 ALTER TABLE `TB_USER` ADD CONSTRAINT `PK_TB_USER` PRIMARY KEY (
-	`U_SEQ`
+        `U_SEQ`
 );
 ALTER TABLE `TB_ORDER` ADD CONSTRAINT `PK_TB_ORDER` PRIMARY KEY (
-	`O_SEQ`
+        `O_SEQ`
 );
 ALTER TABLE `TB_USER_ORDER` ADD CONSTRAINT `PK_TB_USER_ORDER` PRIMARY KEY (
-	`UO_SEQ`
+        `UO_SEQ`
 );
 ALTER TABLE `TB_RESTAURANT` ADD CONSTRAINT `PK_TB_RESTAURANT` PRIMARY KEY (
-	`R_SEQ`
+        `R_SEQ`
 );
 ALTER TABLE `TB_MENU` ADD CONSTRAINT `PK_TB_MENU` PRIMARY KEY (
-	`M_SEQ`
+        `M_SEQ`
 );
 ALTER TABLE `TB_REVIEW` ADD CONSTRAINT `PK_TB_REVIEW` PRIMARY KEY (
-	`RV_SEQ`
+        `RV_SEQ`
 );
 ALTER TABLE `TB_COMMENT` ADD CONSTRAINT `PK_TB_COMMENT` PRIMARY KEY (
-	`C_SEQ`
+        `C_SEQ`
 );
 ALTER TABLE `TB_ORDER` ADD CONSTRAINT `FK_TB_RESTAURANT_TO_TB_ORDER_1` FOREIGN KEY (
-	`R_SEQ`
+        `R_SEQ`
 )
 REFERENCES `TB_RESTAURANT` (
-	`R_SEQ`
+        `R_SEQ`
 );
 ALTER TABLE `TB_USER_ORDER` ADD CONSTRAINT `FK_TB_USER_TO_TB_USER_ORDER_1` FOREIGN KEY (
-	`U_SEQ`
+        `U_SEQ`
 )
 REFERENCES `TB_USER` (
-	`U_SEQ`
+        `U_SEQ`
 );
 ALTER TABLE `TB_USER_ORDER` ADD CONSTRAINT `FK_TB_ORDER_TO_TB_USER_ORDER_1` FOREIGN KEY (
-	`O_SEQ`
+        `O_SEQ`
 )
 REFERENCES `TB_ORDER` (
-	`O_SEQ`
+        `O_SEQ`
 );
 ALTER TABLE `TB_USER_ORDER` ADD CONSTRAINT `FK_TB_MENU_TO_TB_USER_ORDER_1` FOREIGN KEY (
-	`M_SEQ`
+        `M_SEQ`
 )
 REFERENCES `TB_MENU` (
-	`M_SEQ`
+        `M_SEQ`
 );
 ALTER TABLE `TB_USER_ORDER` ADD CONSTRAINT `FK_TB_REVIEW_TO_TB_USER_ORDER_1` FOREIGN KEY (
-	`RV_SEQ`
+        `RV_SEQ`
 )
 REFERENCES `TB_REVIEW` (
-	`RV_SEQ`
+        `RV_SEQ`
 );
 ALTER TABLE `TB_MENU` ADD CONSTRAINT `FK_TB_RESTAURANT_TO_TB_MENU_1` FOREIGN KEY (
-	`R_SEQ`
+        `R_SEQ`
 )
 REFERENCES `TB_RESTAURANT` (
-	`R_SEQ`
+        `R_SEQ`
 );
 ALTER TABLE `TB_REVIEW` ADD CONSTRAINT `FK_TB_MENU_TO_TB_REVIEW_1` FOREIGN KEY (
-	`M_SEQ`
+        `M_SEQ`
 )
 REFERENCES `TB_MENU` (
-	`M_SEQ`
+        `M_SEQ`
 );
 ALTER TABLE `TB_COMMENT` ADD CONSTRAINT `FK_TB_USER_TO_TB_COMMENT_1` FOREIGN KEY (
-	`U_SEQ`
+        `U_SEQ`
 )
 REFERENCES `TB_USER` (
-	`U_SEQ`
+        `U_SEQ`
 );
 ALTER TABLE `TB_COMMENT` ADD CONSTRAINT `FK_TB_ORDER_TO_TB_COMMENT_1` FOREIGN KEY (
-	`O_SEQ`
+        `O_SEQ`
 )
 REFERENCES `TB_ORDER` (
-	`O_SEQ`
+        `O_SEQ`
 );
 </t>
   </si>
@@ -254,6 +355,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -480,6 +585,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[#9] update ERD.xlsx for DDL changed by created_time column
</commit_message>
<xml_diff>
--- a/Docs/DB/ERD.xlsx
+++ b/Docs/DB/ERD.xlsx
@@ -4,8 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ERD 1.0.0" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DDL 1.0.1" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="DDL 1.0.0" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="DDL 1.0.2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DDL 1.0.1" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="DDL 1.0.0" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,9 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>CREATE TABLE `tb_comment` (
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+  <si>
+    <t>변경 사유</t>
+  </si>
+  <si>
+    <t>CREATED_TIME 반영</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_comment definition
+CREATE TABLE `tb_comment` (
   `C_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '댓글 SEQ',
   `COMMENT` varchar(1000) DEFAULT NULL COMMENT '댓글 내용',
   `P_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '대댓글 용 부모 ID,\r\nNULL : 원글\r\nNOT NULL : 부모 댓글 SEQ',
@@ -38,6 +46,7 @@
   `PRICE` mediumint(8) unsigned NOT NULL DEFAULT '0' COMMENT '메뉴 가격',
   `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
   `R_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '식당 SEQ',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
   PRIMARY KEY (`M_SEQ`),
   KEY `FK_TB_RESTAURANT_TO_TB_MENU_1` (`R_SEQ`),
   CONSTRAINT `FK_TB_RESTAURANT_TO_TB_MENU_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
@@ -67,6 +76,7 @@
   `TEL` varchar(100) DEFAULT NULL COMMENT '식당 전화번호',
   `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
   `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\nETC : 기타, 없음',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
   PRIMARY KEY (`R_SEQ`)
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
   </si>
@@ -90,8 +100,9 @@
   `U_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 시퀀스 ID',
   `NICKNAME` varchar(100) DEFAULT NULL COMMENT '사용자 닉네임',
   `IP` varchar(100) DEFAULT NULL COMMENT 'IP 주소',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
   PRIMARY KEY (`U_SEQ`)
-) ENGINE=InnoDB AUTO_INCREMENT=2 DEFAULT CHARSET=utf8;</t>
+) ENGINE=InnoDB AUTO_INCREMENT=5 DEFAULT CHARSET=utf8;</t>
   </si>
   <si>
     <t>-- yagola.tb_user_order definition
@@ -113,6 +124,56 @@
   CONSTRAINT `FK_TB_REVIEW_TO_TB_USER_ORDER_1` FOREIGN KEY (`RV_SEQ`) REFERENCES `tb_review` (`RV_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
   CONSTRAINT `FK_TB_USER_TO_TB_USER_ORDER_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_comment` (
+  `C_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '댓글 SEQ',
+  `COMMENT` varchar(1000) DEFAULT NULL COMMENT '댓글 내용',
+  `P_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '대댓글 용 부모 ID,\r\nNULL : 원글\r\nNOT NULL : 부모 댓글 SEQ',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  `VIEW` tinyint(1) NOT NULL DEFAULT '0' COMMENT '노출, 미사용 FLAG\r\n0 : 비노출, 미사용, False\r\n1 : 노출, 사용, True',
+  `U_SEQ` mediumint(9) unsigned NOT NULL COMMENT '사용자 시퀀스 ID',
+  `O_SEQ` mediumint(9) unsigned NOT NULL COMMENT '주문 시퀀스',
+  PRIMARY KEY (`C_SEQ`),
+  KEY `FK_TB_ORDER_TO_TB_COMMENT_1` (`O_SEQ`),
+  KEY `FK_TB_USER_TO_TB_COMMENT_1` (`U_SEQ`),
+  CONSTRAINT `FK_TB_ORDER_TO_TB_COMMENT_1` FOREIGN KEY (`O_SEQ`) REFERENCES `tb_order` (`O_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_USER_TO_TB_COMMENT_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_menu definition
+CREATE TABLE `tb_menu` (
+  `M_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '메뉴 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '메뉴 이름',
+  `PRICE` mediumint(8) unsigned NOT NULL DEFAULT '0' COMMENT '메뉴 가격',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `R_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '식당 SEQ',
+  PRIMARY KEY (`M_SEQ`),
+  KEY `FK_TB_RESTAURANT_TO_TB_MENU_1` (`R_SEQ`),
+  CONSTRAINT `FK_TB_RESTAURANT_TO_TB_MENU_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_restaurant definition
+CREATE TABLE `tb_restaurant` (
+  `R_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '식당 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '식당 이름',
+  `API_ID` varchar(100) DEFAULT NULL COMMENT '요기요 API 식당 식별 ID',
+  `TEL` varchar(100) DEFAULT NULL COMMENT '식당 전화번호',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\nETC : 기타, 없음',
+  PRIMARY KEY (`R_SEQ`)
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_user definition
+CREATE TABLE `tb_user` (
+  `U_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 시퀀스 ID',
+  `NICKNAME` varchar(100) DEFAULT NULL COMMENT '사용자 닉네임',
+  `IP` varchar(100) DEFAULT NULL COMMENT 'IP 주소',
+  PRIMARY KEY (`U_SEQ`)
+) ENGINE=InnoDB AUTO_INCREMENT=2 DEFAULT CHARSET=utf8;</t>
   </si>
   <si>
     <t xml:space="preserve">DROP TABLE IF EXISTS `TB_USER`;
@@ -359,6 +420,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -580,39 +645,47 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -632,7 +705,57 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#9] update ddl in ERD for FK not null constraint
</commit_message>
<xml_diff>
--- a/Docs/DB/ERD.xlsx
+++ b/Docs/DB/ERD.xlsx
@@ -4,9 +4,10 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ERD 1.0.0" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DDL 1.0.2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="DDL 1.0.1" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="DDL 1.0.0" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="DDL 1.0.3" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DDL 1.0.2" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="DDL 1.0.1" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="DDL 1.0.0" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>변경 사유</t>
   </si>
   <si>
-    <t>CREATED_TIME 반영</t>
+    <t>FK NOT NULL 재 반영</t>
   </si>
   <si>
     <t>-- yagola.tb_comment definition
@@ -39,6 +40,92 @@
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
   </si>
   <si>
+    <t>CREATE TABLE `tb_menu` (
+  `M_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '메뉴 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '메뉴 이름',
+  `PRICE` mediumint(8) unsigned NOT NULL DEFAULT '0' COMMENT '메뉴 가격',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `R_SEQ` mediumint(9) unsigned NOT NULL COMMENT '식당 SEQ',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  PRIMARY KEY (`M_SEQ`),
+  KEY `FK_TB_RESTAURANT_TO_TB_MENU_1` (`R_SEQ`),
+  CONSTRAINT `FK_TB_RESTAURANT_TO_TB_MENU_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_order` (
+  `O_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '주문 시퀀스',
+  `STATUS` enum('ONLINE','OFFLINE','ORDER','ARRIVAL') NOT NULL DEFAULT 'ONLINE' COMMENT '주문 상태, ONLINE : 참여 가능, OFFLINE : 참여 마감, ORDER : 주문 진행, ARRIVAL : 도착 완료',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '주문 생성 일자',
+  `OFFLINE_TIME` timestamp NULL DEFAULT NULL COMMENT '마감 상태(OFFLINE ) 일자',
+  `ORDER_TIME` timestamp NULL DEFAULT NULL COMMENT '주문 상태(ORDER) 일자',
+  `ARRIVAL_TIME` timestamp NULL DEFAULT NULL COMMENT '도착 상태(ARRIVAL) 일자',
+  `R_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '식당 SEQ',
+  PRIMARY KEY (`O_SEQ`),
+  KEY `FK_TB_RESTAURANT_TO_TB_ORDER_1` (`R_SEQ`),
+  CONSTRAINT `FK_TB_RESTAURANT_TO_TB_ORDER_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB AUTO_INCREMENT=3 DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_restaurant definition
+CREATE TABLE `tb_restaurant` (
+  `R_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '식당 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '식당 이름',
+  `API_ID` varchar(100) DEFAULT NULL COMMENT '요기요 API 식당 식별 ID',
+  `TEL` varchar(100) DEFAULT NULL COMMENT '식당 전화번호',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\nETC : 기타, 없음',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  PRIMARY KEY (`R_SEQ`)
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_review` (
+  `RV_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '후기 SEQ',
+  `LIKE` tinyint(1) NOT NULL DEFAULT '0' COMMENT '좋아요 FLAG\r\n0 : 싫어요, False\r\n1 : 좋아요, True',
+  `COMMENT` varchar(1000) DEFAULT NULL COMMENT '후기 내용',
+  `VIEW` tinyint(1) NOT NULL DEFAULT '0' COMMENT '노출, 미사용 FLAG\r\n0 : 비노출, 미사용, False\r\n1 : 노출, 사용, True',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성일자',
+  `M_SEQ` mediumint(9) unsigned NOT NULL COMMENT '메뉴 SEQ',
+  PRIMARY KEY (`RV_SEQ`),
+  KEY `FK_TB_MENU_TO_TB_REVIEW_1` (`M_SEQ`),
+  CONSTRAINT `FK_TB_MENU_TO_TB_REVIEW_1` FOREIGN KEY (`M_SEQ`) REFERENCES `tb_menu` (`M_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_user definition
+CREATE TABLE `tb_user` (
+  `U_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 시퀀스 ID',
+  `NICKNAME` varchar(100) DEFAULT NULL COMMENT '사용자 닉네임',
+  `IP` varchar(100) DEFAULT NULL COMMENT 'IP 주소',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  PRIMARY KEY (`U_SEQ`)
+) ENGINE=InnoDB AUTO_INCREMENT=5 DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_user_order` (
+  `UO_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 주문 SEQ',
+  `U_SEQ` mediumint(9) unsigned NOT NULL COMMENT '사용자 시퀀스 ID',
+  `O_SEQ` mediumint(9) unsigned NOT NULL COMMENT '주문 시퀀스',
+  `HOST` tinyint(1) NOT NULL DEFAULT '0' COMMENT '원글 작성자 여부 FLAG\r\n0 : 참여자, False\r\n1 : 작성자, True',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  `M_SEQ` mediumint(9) unsigned NOT NULL COMMENT '메뉴 SEQ',
+  `RV_SEQ` mediumint(9) unsigned NOT NULL COMMENT '후기 SEQ',
+  PRIMARY KEY (`UO_SEQ`),
+  KEY `FK_TB_REVIEW_TO_TB_USER_ORDER_1` (`RV_SEQ`),
+  KEY `FK_TB_MENU_TO_TB_USER_ORDER_1` (`M_SEQ`),
+  KEY `FK_TB_ORDER_TO_TB_USER_ORDER_1` (`O_SEQ`),
+  KEY `FK_TB_USER_TO_TB_USER_ORDER_1` (`U_SEQ`),
+  CONSTRAINT `FK_TB_MENU_TO_TB_USER_ORDER_1` FOREIGN KEY (`M_SEQ`) REFERENCES `tb_menu` (`M_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_ORDER_TO_TB_USER_ORDER_1` FOREIGN KEY (`O_SEQ`) REFERENCES `tb_order` (`O_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_REVIEW_TO_TB_USER_ORDER_1` FOREIGN KEY (`RV_SEQ`) REFERENCES `tb_review` (`RV_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_USER_TO_TB_USER_ORDER_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
+    <t>CREATED_TIME 반영</t>
+  </si>
+  <si>
     <t>-- yagola.tb_menu definition
 CREATE TABLE `tb_menu` (
   `M_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '메뉴 SEQ',
@@ -68,19 +155,6 @@
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
   </si>
   <si>
-    <t>-- yagola.tb_restaurant definition
-CREATE TABLE `tb_restaurant` (
-  `R_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '식당 SEQ',
-  `NAME` varchar(100) DEFAULT NULL COMMENT '식당 이름',
-  `API_ID` varchar(100) DEFAULT NULL COMMENT '요기요 API 식당 식별 ID',
-  `TEL` varchar(100) DEFAULT NULL COMMENT '식당 전화번호',
-  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
-  `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\nETC : 기타, 없음',
-  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
-  PRIMARY KEY (`R_SEQ`)
-) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
-  </si>
-  <si>
     <t>-- yagola.tb_review definition
 CREATE TABLE `tb_review` (
   `RV_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '후기 SEQ',
@@ -93,16 +167,6 @@
   KEY `FK_TB_MENU_TO_TB_REVIEW_1` (`M_SEQ`),
   CONSTRAINT `FK_TB_MENU_TO_TB_REVIEW_1` FOREIGN KEY (`M_SEQ`) REFERENCES `tb_menu` (`M_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
-  </si>
-  <si>
-    <t>-- yagola.tb_user definition
-CREATE TABLE `tb_user` (
-  `U_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 시퀀스 ID',
-  `NICKNAME` varchar(100) DEFAULT NULL COMMENT '사용자 닉네임',
-  `IP` varchar(100) DEFAULT NULL COMMENT 'IP 주소',
-  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
-  PRIMARY KEY (`U_SEQ`)
-) ENGINE=InnoDB AUTO_INCREMENT=5 DEFAULT CHARSET=utf8;</t>
   </si>
   <si>
     <t>-- yagola.tb_user_order definition
@@ -424,6 +488,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -703,19 +771,22 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -725,7 +796,7 @@
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -735,7 +806,12 @@
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +831,57 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#28] add joinOrder / DDL add / add UserOrderDTO
</commit_message>
<xml_diff>
--- a/Docs/DB/ERD.xlsx
+++ b/Docs/DB/ERD.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yagola\Docs\DB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74DEA26-6501-4EA1-BB56-30DE8EF349AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-25560" yWindow="750" windowWidth="21600" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="ERD 1.0.0" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DDL 1.0.3" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="DDL 1.0.2" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="DDL 1.0.1" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="DDL 1.0.0" sheetId="5" r:id="rId8"/>
+    <sheet name="ERD 1.0.0" sheetId="1" r:id="rId1"/>
+    <sheet name="DDL 1.0.4" sheetId="6" r:id="rId2"/>
+    <sheet name="DDL 1.0.3" sheetId="2" r:id="rId3"/>
+    <sheet name="DDL 1.0.2" sheetId="3" r:id="rId4"/>
+    <sheet name="DDL 1.0.1" sheetId="4" r:id="rId5"/>
+    <sheet name="DDL 1.0.0" sheetId="5" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>변경 사유</t>
   </si>
@@ -401,20 +411,174 @@
 );
 </t>
   </si>
+  <si>
+    <r>
+      <t>ALTER TABLE yagola.tb_order ADD U_SEQ mediumint unsigned NULL COMMENT '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>유저</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> SEQ';</t>
+    </r>
+  </si>
+  <si>
+    <t>ALTER TABLE yagola.tb_order ADD CONSTRAINT FK_TB_USER_TO_TB_ORDER_1 FOREIGN KEY (U_SEQ) REFERENCES yagola.tb_user(U_SEQ) ON DELETE CASCADE ON UPDATE CASCADE;</t>
+  </si>
+  <si>
+    <t>변경 사유</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">order </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">테이블에 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">user </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>정보 추가</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>ALTER TABLE yagola.tb_user_order MODIFY COLUMN RV_SEQ mediumint unsigned NULL COMMENT '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>후기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> SEQ';</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>userorder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">에 리뷰가 없을 수도 있으므로 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">not null </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -422,32 +586,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -458,11 +635,17 @@
     <xdr:ext cx="13687425" cy="6819900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="이미지"/>
+        <xdr:cNvPr id="2" name="image1.png" title="이미지">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -479,24 +662,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -686,205 +853,271 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996F44BF-6C9A-4796-87D0-904D5C4324CF}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="1" t="s">
-        <v>8</v>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2">
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2">
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2">
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
+    <row r="8" spans="1:2">
       <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:2">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetData>
+    <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[#9] change DDL add CATEGORY CHICKEN in RESTAURANT
</commit_message>
<xml_diff>
--- a/Docs/DB/ERD.xlsx
+++ b/Docs/DB/ERD.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ERD 1.0.0" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DDL 1.0.3" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="DDL 1.0.2" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="DDL 1.0.1" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="DDL 1.0.0" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="DDL 1.0.4" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DDL 1.0.3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="DDL 1.0.2" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="DDL 1.0.1" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="DDL 1.0.0" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>변경 사유</t>
   </si>
@@ -67,17 +68,16 @@
 ) ENGINE=InnoDB AUTO_INCREMENT=3 DEFAULT CHARSET=utf8</t>
   </si>
   <si>
-    <t>-- yagola.tb_restaurant definition
-CREATE TABLE `tb_restaurant` (
+    <t>CREATE TABLE `tb_restaurant` (
   `R_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '식당 SEQ',
   `NAME` varchar(100) DEFAULT NULL COMMENT '식당 이름',
   `API_ID` varchar(100) DEFAULT NULL COMMENT '요기요 API 식당 식별 ID',
   `TEL` varchar(100) DEFAULT NULL COMMENT '식당 전화번호',
   `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
-  `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\nETC : 기타, 없음',
+  `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','CHICKEN','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\n CHICKEN: 치킨 ETC : 기타, 없음',
   `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
   PRIMARY KEY (`R_SEQ`)
-) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+) ENGINE=InnoDB AUTO_INCREMENT=3 DEFAULT CHARSET=utf8</t>
   </si>
   <si>
     <t>CREATE TABLE `tb_review` (
@@ -121,6 +121,19 @@
   CONSTRAINT `FK_TB_REVIEW_TO_TB_USER_ORDER_1` FOREIGN KEY (`RV_SEQ`) REFERENCES `tb_review` (`RV_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
   CONSTRAINT `FK_TB_USER_TO_TB_USER_ORDER_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_restaurant definition
+CREATE TABLE `tb_restaurant` (
+  `R_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '식당 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '식당 이름',
+  `API_ID` varchar(100) DEFAULT NULL COMMENT '요기요 API 식당 식별 ID',
+  `TEL` varchar(100) DEFAULT NULL COMMENT '식당 전화번호',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `CATEGORY` enum('CHINA','KOREA','JAPAN','ALONE','FRANCHISE','WESTERN','PIG','NIGHT','SCHOOL','CAFE','MART','ETC') DEFAULT 'ETC' COMMENT '식당 카테고리\r\nCHINA : 중식\r\nKOREA : 한식\r\nJAPAN : 일식/돈까스\r\nALONE : 1인분\r\nFRANCHISE : 프랜차이즈\r\nWESTERN : 피자/양식\r\nPIG : 족발/보쌈\r\nNIGHT : 야식\r\nSCHOOL : 분식\r\nCAFE : 카페/디저트\r\nMART : 편의점/마트\r\nETC : 기타, 없음',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  PRIMARY KEY (`R_SEQ`)
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
   </si>
   <si>
     <t>CREATED_TIME 반영</t>
@@ -492,6 +505,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -776,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -786,22 +803,22 @@
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -811,7 +828,7 @@
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -829,14 +846,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1" t="s">
-        <v>14</v>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -846,22 +866,27 @@
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -881,7 +906,57 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#9] update DDL for Batch with init Batch Config Table
</commit_message>
<xml_diff>
--- a/Docs/DB/ERD.xlsx
+++ b/Docs/DB/ERD.xlsx
@@ -4,11 +4,12 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ERD 1.0.0" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DDL 1.0.4" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="DDL 1.0.3" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="DDL 1.0.2" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="DDL 1.0.1" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="DDL 1.0.0" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="DDL 1.1.0" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DDL 1.0.4" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="DDL 1.0.3" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="DDL 1.0.2" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="DDL 1.0.1" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="DDL 1.0.0" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,12 +17,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
-  <si>
-    <t>변경 사유</t>
-  </si>
-  <si>
-    <t>FK NOT NULL 재 반영</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+  <si>
+    <t>변경사유</t>
+  </si>
+  <si>
+    <t>Batch Config Table 추가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CREATE TABLE BATCH_JOB_INSTANCE  (
+        JOB_INSTANCE_ID BIGINT  NOT NULL PRIMARY KEY ,
+        VERSION BIGINT ,
+        JOB_NAME VARCHAR(100) NOT NULL,
+        JOB_KEY VARCHAR(32) NOT NULL,
+        constraint JOB_INST_UN unique (JOB_NAME, JOB_KEY)
+) ENGINE=InnoDB;
+CREATE TABLE BATCH_JOB_EXECUTION  (
+        JOB_EXECUTION_ID BIGINT  NOT NULL PRIMARY KEY ,
+        VERSION BIGINT  ,
+        JOB_INSTANCE_ID BIGINT NOT NULL,
+        CREATE_TIME DATETIME(6) NOT NULL,
+        START_TIME DATETIME(6) DEFAULT NULL ,
+        END_TIME DATETIME(6) DEFAULT NULL ,
+        STATUS VARCHAR(10) ,
+        EXIT_CODE VARCHAR(2500) ,
+        EXIT_MESSAGE VARCHAR(2500) ,
+        LAST_UPDATED DATETIME(6),
+        constraint JOB_INST_EXEC_FK foreign key (JOB_INSTANCE_ID)
+        references BATCH_JOB_INSTANCE(JOB_INSTANCE_ID)
+) ENGINE=InnoDB;
+CREATE TABLE BATCH_JOB_EXECUTION_PARAMS  (
+        JOB_EXECUTION_ID BIGINT NOT NULL ,
+        TYPE_CD VARCHAR(6) NOT NULL ,
+        KEY_NAME VARCHAR(100) NOT NULL ,
+        STRING_VAL VARCHAR(250) ,
+        DATE_VAL DATETIME(6) DEFAULT NULL ,
+        LONG_VAL BIGINT ,
+        DOUBLE_VAL DOUBLE PRECISION ,
+        IDENTIFYING CHAR(1) NOT NULL ,
+        constraint JOB_EXEC_PARAMS_FK foreign key (JOB_EXECUTION_ID)
+        references BATCH_JOB_EXECUTION(JOB_EXECUTION_ID)
+) ENGINE=InnoDB;
+CREATE TABLE BATCH_STEP_EXECUTION  (
+        STEP_EXECUTION_ID BIGINT  NOT NULL PRIMARY KEY ,
+        VERSION BIGINT NOT NULL,
+        STEP_NAME VARCHAR(100) NOT NULL,
+        JOB_EXECUTION_ID BIGINT NOT NULL,
+        START_TIME DATETIME(6) NOT NULL ,
+        END_TIME DATETIME(6) DEFAULT NULL ,
+        STATUS VARCHAR(10) ,
+        COMMIT_COUNT BIGINT ,
+        READ_COUNT BIGINT ,
+        FILTER_COUNT BIGINT ,
+        WRITE_COUNT BIGINT ,
+        READ_SKIP_COUNT BIGINT ,
+        WRITE_SKIP_COUNT BIGINT ,
+        PROCESS_SKIP_COUNT BIGINT ,
+        ROLLBACK_COUNT BIGINT ,
+        EXIT_CODE VARCHAR(2500) ,
+        EXIT_MESSAGE VARCHAR(2500) ,
+        LAST_UPDATED DATETIME(6),
+        constraint JOB_EXEC_STEP_FK foreign key (JOB_EXECUTION_ID)
+        references BATCH_JOB_EXECUTION(JOB_EXECUTION_ID)
+) ENGINE=InnoDB;
+CREATE TABLE BATCH_STEP_EXECUTION_CONTEXT  (
+        STEP_EXECUTION_ID BIGINT NOT NULL PRIMARY KEY,
+        SHORT_CONTEXT VARCHAR(2500) NOT NULL,
+        SERIALIZED_CONTEXT TEXT ,
+        constraint STEP_EXEC_CTX_FK foreign key (STEP_EXECUTION_ID)
+        references BATCH_STEP_EXECUTION(STEP_EXECUTION_ID)
+) ENGINE=InnoDB;
+CREATE TABLE BATCH_JOB_EXECUTION_CONTEXT  (
+        JOB_EXECUTION_ID BIGINT NOT NULL PRIMARY KEY,
+        SHORT_CONTEXT VARCHAR(2500) NOT NULL,
+        SERIALIZED_CONTEXT TEXT ,
+        constraint JOB_EXEC_CTX_FK foreign key (JOB_EXECUTION_ID)
+        references BATCH_JOB_EXECUTION(JOB_EXECUTION_ID)
+) ENGINE=InnoDB;
+CREATE TABLE BATCH_STEP_EXECUTION_SEQ (
+        ID BIGINT NOT NULL,
+        UNIQUE_KEY CHAR(1) NOT NULL,
+        constraint UNIQUE_KEY_UN unique (UNIQUE_KEY)
+) ENGINE=InnoDB;
+INSERT INTO BATCH_STEP_EXECUTION_SEQ (ID, UNIQUE_KEY) select * from (select 0 as ID, '0' as UNIQUE_KEY) as tmp where not exists(select * from BATCH_STEP_EXECUTION_SEQ);
+CREATE TABLE BATCH_JOB_EXECUTION_SEQ (
+        ID BIGINT NOT NULL,
+        UNIQUE_KEY CHAR(1) NOT NULL,
+        constraint UNIQUE_KEY_UN unique (UNIQUE_KEY)
+) ENGINE=InnoDB;
+INSERT INTO BATCH_JOB_EXECUTION_SEQ (ID, UNIQUE_KEY) select * from (select 0 as ID, '0' as UNIQUE_KEY) as tmp where not exists(select * from BATCH_JOB_EXECUTION_SEQ);
+CREATE TABLE BATCH_JOB_SEQ (
+        ID BIGINT NOT NULL,
+        UNIQUE_KEY CHAR(1) NOT NULL,
+        constraint UNIQUE_KEY_UN unique (UNIQUE_KEY)
+) ENGINE=InnoDB;
+INSERT INTO BATCH_JOB_SEQ (ID, UNIQUE_KEY) select * from (select 0 as ID, '0' as UNIQUE_KEY) as tmp where not exists(select * from BATCH_JOB_SEQ);</t>
   </si>
   <si>
     <t>-- yagola.tb_comment definition
@@ -123,6 +214,56 @@
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
   </si>
   <si>
+    <t>변경 사유</t>
+  </si>
+  <si>
+    <t>FK NOT NULL 재 반영</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_comment definition
+CREATE TABLE `tb_comment` (
+  `C_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '댓글 SEQ',
+  `COMMENT` varchar(1000) DEFAULT NULL COMMENT '댓글 내용',
+  `P_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '대댓글 용 부모 ID,\r\nNULL : 원글\r\nNOT NULL : 부모 댓글 SEQ',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  `VIEW` tinyint(1) NOT NULL DEFAULT '0' COMMENT '노출, 미사용 FLAG\r\n0 : 비노출, 미사용, False\r\n1 : 노출, 사용, True',
+  `U_SEQ` mediumint(9) unsigned NOT NULL COMMENT '사용자 시퀀스 ID',
+  `O_SEQ` mediumint(9) unsigned NOT NULL COMMENT '주문 시퀀스',
+  PRIMARY KEY (`C_SEQ`),
+  KEY `FK_TB_ORDER_TO_TB_COMMENT_1` (`O_SEQ`),
+  KEY `FK_TB_USER_TO_TB_COMMENT_1` (`U_SEQ`),
+  CONSTRAINT `FK_TB_ORDER_TO_TB_COMMENT_1` FOREIGN KEY (`O_SEQ`) REFERENCES `tb_order` (`O_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_USER_TO_TB_COMMENT_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_menu` (
+  `M_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '메뉴 SEQ',
+  `NAME` varchar(100) DEFAULT NULL COMMENT '메뉴 이름',
+  `PRICE` mediumint(8) unsigned NOT NULL DEFAULT '0' COMMENT '메뉴 가격',
+  `IMG_LINK` varchar(512) DEFAULT NULL COMMENT '요기요 이미지 Link 주소',
+  `R_SEQ` mediumint(9) unsigned NOT NULL COMMENT '식당 SEQ',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  PRIMARY KEY (`M_SEQ`),
+  KEY `FK_TB_RESTAURANT_TO_TB_MENU_1` (`R_SEQ`),
+  CONSTRAINT `FK_TB_RESTAURANT_TO_TB_MENU_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_order` (
+  `O_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '주문 시퀀스',
+  `STATUS` enum('ONLINE','OFFLINE','ORDER','ARRIVAL') NOT NULL DEFAULT 'ONLINE' COMMENT '주문 상태, ONLINE : 참여 가능, OFFLINE : 참여 마감, ORDER : 주문 진행, ARRIVAL : 도착 완료',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '주문 생성 일자',
+  `OFFLINE_TIME` timestamp NULL DEFAULT NULL COMMENT '마감 상태(OFFLINE ) 일자',
+  `ORDER_TIME` timestamp NULL DEFAULT NULL COMMENT '주문 상태(ORDER) 일자',
+  `ARRIVAL_TIME` timestamp NULL DEFAULT NULL COMMENT '도착 상태(ARRIVAL) 일자',
+  `R_SEQ` mediumint(9) unsigned DEFAULT NULL COMMENT '식당 SEQ',
+  PRIMARY KEY (`O_SEQ`),
+  KEY `FK_TB_RESTAURANT_TO_TB_ORDER_1` (`R_SEQ`),
+  CONSTRAINT `FK_TB_RESTAURANT_TO_TB_ORDER_1` FOREIGN KEY (`R_SEQ`) REFERENCES `tb_restaurant` (`R_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB AUTO_INCREMENT=3 DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
     <t>-- yagola.tb_restaurant definition
 CREATE TABLE `tb_restaurant` (
   `R_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '식당 SEQ',
@@ -134,6 +275,49 @@
   `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
   PRIMARY KEY (`R_SEQ`)
 ) ENGINE=InnoDB DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_review` (
+  `RV_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '후기 SEQ',
+  `LIKE` tinyint(1) NOT NULL DEFAULT '0' COMMENT '좋아요 FLAG\r\n0 : 싫어요, False\r\n1 : 좋아요, True',
+  `COMMENT` varchar(1000) DEFAULT NULL COMMENT '후기 내용',
+  `VIEW` tinyint(1) NOT NULL DEFAULT '0' COMMENT '노출, 미사용 FLAG\r\n0 : 비노출, 미사용, False\r\n1 : 노출, 사용, True',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성일자',
+  `M_SEQ` mediumint(9) unsigned NOT NULL COMMENT '메뉴 SEQ',
+  PRIMARY KEY (`RV_SEQ`),
+  KEY `FK_TB_MENU_TO_TB_REVIEW_1` (`M_SEQ`),
+  CONSTRAINT `FK_TB_MENU_TO_TB_REVIEW_1` FOREIGN KEY (`M_SEQ`) REFERENCES `tb_menu` (`M_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
+  </si>
+  <si>
+    <t>-- yagola.tb_user definition
+CREATE TABLE `tb_user` (
+  `U_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 시퀀스 ID',
+  `NICKNAME` varchar(100) DEFAULT NULL COMMENT '사용자 닉네임',
+  `IP` varchar(100) DEFAULT NULL COMMENT 'IP 주소',
+  `CREATED_TIME` timestamp NOT NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  PRIMARY KEY (`U_SEQ`)
+) ENGINE=InnoDB AUTO_INCREMENT=5 DEFAULT CHARSET=utf8;</t>
+  </si>
+  <si>
+    <t>CREATE TABLE `tb_user_order` (
+  `UO_SEQ` mediumint(9) unsigned NOT NULL AUTO_INCREMENT COMMENT '사용자 주문 SEQ',
+  `U_SEQ` mediumint(9) unsigned NOT NULL COMMENT '사용자 시퀀스 ID',
+  `O_SEQ` mediumint(9) unsigned NOT NULL COMMENT '주문 시퀀스',
+  `HOST` tinyint(1) NOT NULL DEFAULT '0' COMMENT '원글 작성자 여부 FLAG\r\n0 : 참여자, False\r\n1 : 작성자, True',
+  `CREATED_TIME` timestamp NULL DEFAULT CURRENT_TIMESTAMP COMMENT '생성 일자',
+  `M_SEQ` mediumint(9) unsigned NOT NULL COMMENT '메뉴 SEQ',
+  `RV_SEQ` mediumint(9) unsigned NOT NULL COMMENT '후기 SEQ',
+  PRIMARY KEY (`UO_SEQ`),
+  KEY `FK_TB_REVIEW_TO_TB_USER_ORDER_1` (`RV_SEQ`),
+  KEY `FK_TB_MENU_TO_TB_USER_ORDER_1` (`M_SEQ`),
+  KEY `FK_TB_ORDER_TO_TB_USER_ORDER_1` (`O_SEQ`),
+  KEY `FK_TB_USER_TO_TB_USER_ORDER_1` (`U_SEQ`),
+  CONSTRAINT `FK_TB_MENU_TO_TB_USER_ORDER_1` FOREIGN KEY (`M_SEQ`) REFERENCES `tb_menu` (`M_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_ORDER_TO_TB_USER_ORDER_1` FOREIGN KEY (`O_SEQ`) REFERENCES `tb_order` (`O_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_REVIEW_TO_TB_USER_ORDER_1` FOREIGN KEY (`RV_SEQ`) REFERENCES `tb_review` (`RV_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE,
+  CONSTRAINT `FK_TB_USER_TO_TB_USER_ORDER_1` FOREIGN KEY (`U_SEQ`) REFERENCES `tb_user` (`U_SEQ`) ON DELETE CASCADE ON UPDATE CASCADE
+) ENGINE=InnoDB DEFAULT CHARSET=utf8</t>
   </si>
   <si>
     <t>CREATED_TIME 반영</t>
@@ -509,6 +693,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -738,39 +926,44 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -790,45 +983,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -848,45 +1041,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -904,39 +1097,47 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -956,7 +1157,57 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>